<commit_message>
Add new file and edit file
</commit_message>
<xml_diff>
--- a/bagging_akurasi.xlsx
+++ b/bagging_akurasi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,95 +434,97 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>k:2</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>k:3</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>k:4</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>k:5</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>k:6</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>k:7</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>k:8</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>k:9</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>k:10</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>k:11</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>k:12</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>k:13</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>k:14</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>k:15</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>fold 1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>70.13</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>66.23</v>
-      </c>
-      <c r="C2" t="n">
-        <v>68.83</v>
       </c>
       <c r="D2" t="n">
         <v>68.83</v>
       </c>
       <c r="E2" t="n">
+        <v>68.83</v>
+      </c>
+      <c r="F2" t="n">
         <v>70.13</v>
-      </c>
-      <c r="F2" t="n">
-        <v>72.73</v>
       </c>
       <c r="G2" t="n">
         <v>72.73</v>
@@ -531,180 +533,200 @@
         <v>72.73</v>
       </c>
       <c r="I2" t="n">
+        <v>72.73</v>
+      </c>
+      <c r="J2" t="n">
         <v>70.13</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>74.03</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>67.53</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>74.03</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>75.31999999999999</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>72.73</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>fold 2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>67.53</v>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>61.04</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>67.53</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>70.13</v>
       </c>
-      <c r="E3" t="n">
-        <v>76.62</v>
-      </c>
       <c r="F3" t="n">
+        <v>76.62</v>
+      </c>
+      <c r="G3" t="n">
         <v>68.83</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>75.31999999999999</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>72.73</v>
-      </c>
-      <c r="I3" t="n">
-        <v>74.03</v>
       </c>
       <c r="J3" t="n">
         <v>74.03</v>
       </c>
       <c r="K3" t="n">
-        <v>76.62</v>
+        <v>74.03</v>
       </c>
       <c r="L3" t="n">
-        <v>75.31999999999999</v>
+        <v>76.62</v>
       </c>
       <c r="M3" t="n">
         <v>75.31999999999999</v>
       </c>
       <c r="N3" t="n">
+        <v>75.31999999999999</v>
+      </c>
+      <c r="O3" t="n">
         <v>66.23</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>fold 3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>77.63</v>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>80.26000000000001</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>76.31999999999999</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>81.58</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>80.26000000000001</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>81.58</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>75</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>82.89</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>80.26000000000001</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>78.95</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>81.58</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>77.63</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>82.89</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>81.58</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>fold 4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>58.44</v>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>71.43000000000001</v>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>72.73</v>
-      </c>
-      <c r="D5" t="n">
-        <v>66.23</v>
       </c>
       <c r="E5" t="n">
         <v>66.23</v>
       </c>
       <c r="F5" t="n">
+        <v>66.23</v>
+      </c>
+      <c r="G5" t="n">
         <v>68.83</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>67.53</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>68.83</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>64.94</v>
       </c>
-      <c r="J5" t="n">
+      <c r="K5" t="n">
         <v>67.53</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>70.13</v>
-      </c>
-      <c r="L5" t="n">
-        <v>67.53</v>
       </c>
       <c r="M5" t="n">
         <v>67.53</v>
       </c>
       <c r="N5" t="n">
+        <v>67.53</v>
+      </c>
+      <c r="O5" t="n">
         <v>68.83</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>fold 5</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>79.22</v>
       </c>
-      <c r="B6" t="n">
+      <c r="C6" t="n">
         <v>80.52</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>81.81999999999999</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>71.43000000000001</v>
-      </c>
-      <c r="E6" t="n">
-        <v>74.03</v>
       </c>
       <c r="F6" t="n">
         <v>74.03</v>
       </c>
       <c r="G6" t="n">
+        <v>74.03</v>
+      </c>
+      <c r="H6" t="n">
         <v>75.31999999999999</v>
-      </c>
-      <c r="H6" t="n">
-        <v>79.22</v>
       </c>
       <c r="I6" t="n">
         <v>79.22</v>
@@ -713,46 +735,51 @@
         <v>79.22</v>
       </c>
       <c r="K6" t="n">
-        <v>76.62</v>
+        <v>79.22</v>
       </c>
       <c r="L6" t="n">
-        <v>77.92</v>
+        <v>76.62</v>
       </c>
       <c r="M6" t="n">
+        <v>77.92</v>
+      </c>
+      <c r="N6" t="n">
         <v>79.22</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>77.92</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>fold 6</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>66.23</v>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>75.31999999999999</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>72.73</v>
       </c>
-      <c r="D7" t="n">
-        <v>76.62</v>
-      </c>
       <c r="E7" t="n">
+        <v>76.62</v>
+      </c>
+      <c r="F7" t="n">
         <v>74.03</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>75.31999999999999</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>71.43000000000001</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>74.03</v>
       </c>
-      <c r="I7" t="n">
-        <v>76.62</v>
-      </c>
       <c r="J7" t="n">
         <v>76.62</v>
       </c>
@@ -760,188 +787,211 @@
         <v>76.62</v>
       </c>
       <c r="L7" t="n">
-        <v>77.92</v>
+        <v>76.62</v>
       </c>
       <c r="M7" t="n">
         <v>77.92</v>
       </c>
       <c r="N7" t="n">
+        <v>77.92</v>
+      </c>
+      <c r="O7" t="n">
         <v>79.22</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>77.92</v>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>fold 7</t>
+        </is>
       </c>
       <c r="B8" t="n">
-        <v>76.62</v>
+        <v>77.92</v>
       </c>
       <c r="C8" t="n">
+        <v>76.62</v>
+      </c>
+      <c r="D8" t="n">
         <v>75.31999999999999</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>79.22</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>72.73</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>79.22</v>
       </c>
-      <c r="G8" t="n">
-        <v>77.92</v>
-      </c>
       <c r="H8" t="n">
-        <v>79.22</v>
+        <v>77.92</v>
       </c>
       <c r="I8" t="n">
         <v>79.22</v>
       </c>
       <c r="J8" t="n">
-        <v>77.92</v>
+        <v>79.22</v>
       </c>
       <c r="K8" t="n">
-        <v>76.62</v>
+        <v>77.92</v>
       </c>
       <c r="L8" t="n">
         <v>76.62</v>
       </c>
       <c r="M8" t="n">
-        <v>77.92</v>
+        <v>76.62</v>
       </c>
       <c r="N8" t="n">
+        <v>77.92</v>
+      </c>
+      <c r="O8" t="n">
         <v>77.92</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>fold 8</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>72.37</v>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>80.26000000000001</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>77.63</v>
-      </c>
-      <c r="D9" t="n">
-        <v>78.95</v>
       </c>
       <c r="E9" t="n">
         <v>78.95</v>
       </c>
       <c r="F9" t="n">
+        <v>78.95</v>
+      </c>
+      <c r="G9" t="n">
         <v>76.31999999999999</v>
-      </c>
-      <c r="G9" t="n">
-        <v>82.89</v>
       </c>
       <c r="H9" t="n">
         <v>82.89</v>
       </c>
       <c r="I9" t="n">
+        <v>82.89</v>
+      </c>
+      <c r="J9" t="n">
         <v>81.58</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>80.26000000000001</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>82.89</v>
       </c>
-      <c r="L9" t="n">
+      <c r="M9" t="n">
         <v>75</v>
-      </c>
-      <c r="M9" t="n">
-        <v>81.58</v>
       </c>
       <c r="N9" t="n">
         <v>81.58</v>
       </c>
+      <c r="O9" t="n">
+        <v>81.58</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>fold 9</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
         <v>67.53</v>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>68.83</v>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>70.13</v>
       </c>
-      <c r="D10" t="n">
-        <v>76.62</v>
-      </c>
       <c r="E10" t="n">
+        <v>76.62</v>
+      </c>
+      <c r="F10" t="n">
         <v>70.13</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>72.73</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>68.83</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>71.43000000000001</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>70.13</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>68.83</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>71.43000000000001</v>
       </c>
-      <c r="L10" t="n">
+      <c r="M10" t="n">
         <v>68.83</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>74.03</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>71.43000000000001</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>fold 10</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>75.31999999999999</v>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>74.03</v>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>79.22</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>75.31999999999999</v>
       </c>
-      <c r="E11" t="n">
-        <v>76.62</v>
-      </c>
       <c r="F11" t="n">
         <v>76.62</v>
       </c>
       <c r="G11" t="n">
+        <v>76.62</v>
+      </c>
+      <c r="H11" t="n">
         <v>81.81999999999999</v>
       </c>
-      <c r="H11" t="n">
-        <v>76.62</v>
-      </c>
       <c r="I11" t="n">
-        <v>77.92</v>
+        <v>76.62</v>
       </c>
       <c r="J11" t="n">
-        <v>76.62</v>
+        <v>77.92</v>
       </c>
       <c r="K11" t="n">
-        <v>77.92</v>
+        <v>76.62</v>
       </c>
       <c r="L11" t="n">
+        <v>77.92</v>
+      </c>
+      <c r="M11" t="n">
         <v>75.31999999999999</v>
       </c>
-      <c r="M11" t="n">
-        <v>76.62</v>
-      </c>
       <c r="N11" t="n">
+        <v>76.62</v>
+      </c>
+      <c r="O11" t="n">
         <v>77.92</v>
       </c>
     </row>

</xml_diff>